<commit_message>
Change engimon sprite in xlsx
</commit_message>
<xml_diff>
--- a/data/Engimon.xlsx
+++ b/data/Engimon.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STEI\Sem4\PBO\Tubes2\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STEI\Sem4\PBO\Nintendont-Game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B373C009-3A16-4AE3-983F-CD5D565F27FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C507E4B9-E491-4B59-9191-0D07DCCFB803}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2220F236-1362-4FC8-8C2A-8F31A1E32F85}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="182">
   <si>
     <t>Name</t>
   </si>
@@ -556,6 +556,30 @@
   </si>
   <si>
     <t>hoho huhu</t>
+  </si>
+  <si>
+    <t>Battle Image</t>
+  </si>
+  <si>
+    <t>Sprite Image</t>
+  </si>
+  <si>
+    <t>Engimon/004.png</t>
+  </si>
+  <si>
+    <t>Engimon/000.png</t>
+  </si>
+  <si>
+    <t>Engimon/007.png</t>
+  </si>
+  <si>
+    <t>Engimon/011.png</t>
+  </si>
+  <si>
+    <t>Engimon/053.png</t>
+  </si>
+  <si>
+    <t>Engimon/333.png</t>
   </si>
 </sst>
 </file>
@@ -907,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAA2AB0-BD4B-4942-9DAC-0BAE7234D902}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,10 +943,12 @@
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" customWidth="1"/>
     <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -938,8 +964,14 @@
       <c r="E1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -955,8 +987,14 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>176</v>
+      </c>
+      <c r="G2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -972,8 +1010,14 @@
       <c r="E3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -989,8 +1033,14 @@
       <c r="E4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>179</v>
+      </c>
+      <c r="G4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1006,8 +1056,14 @@
       <c r="E5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1023,8 +1079,14 @@
       <c r="E6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>178</v>
+      </c>
+      <c r="G6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1040,8 +1102,14 @@
       <c r="E7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1057,8 +1125,14 @@
       <c r="E8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>177</v>
+      </c>
+      <c r="G8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -1074,8 +1148,14 @@
       <c r="E9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1091,8 +1171,14 @@
       <c r="E10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>177</v>
+      </c>
+      <c r="G10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1108,8 +1194,14 @@
       <c r="E11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1125,8 +1217,14 @@
       <c r="E12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>177</v>
+      </c>
+      <c r="G12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1142,8 +1240,14 @@
       <c r="E13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>177</v>
+      </c>
+      <c r="G13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -1159,8 +1263,14 @@
       <c r="E14" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>177</v>
+      </c>
+      <c r="G14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -1176,8 +1286,14 @@
       <c r="E15" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>177</v>
+      </c>
+      <c r="G15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -1193,8 +1309,14 @@
       <c r="E16" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>177</v>
+      </c>
+      <c r="G16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -1210,8 +1332,14 @@
       <c r="E17" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>177</v>
+      </c>
+      <c r="G17" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -1227,8 +1355,14 @@
       <c r="E18" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>177</v>
+      </c>
+      <c r="G18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -1244,8 +1378,14 @@
       <c r="E19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>177</v>
+      </c>
+      <c r="G19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -1261,8 +1401,14 @@
       <c r="E20" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>177</v>
+      </c>
+      <c r="G20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -1278,8 +1424,14 @@
       <c r="E21" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>177</v>
+      </c>
+      <c r="G21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>98</v>
       </c>
@@ -1295,8 +1447,14 @@
       <c r="E22" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>177</v>
+      </c>
+      <c r="G22" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>102</v>
       </c>
@@ -1312,8 +1470,14 @@
       <c r="E23" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>177</v>
+      </c>
+      <c r="G23" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>106</v>
       </c>
@@ -1329,8 +1493,14 @@
       <c r="E24" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>177</v>
+      </c>
+      <c r="G24" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>111</v>
       </c>
@@ -1346,8 +1516,14 @@
       <c r="E25" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>177</v>
+      </c>
+      <c r="G25" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>116</v>
       </c>
@@ -1363,8 +1539,14 @@
       <c r="E26" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>177</v>
+      </c>
+      <c r="G26" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>121</v>
       </c>
@@ -1380,8 +1562,14 @@
       <c r="E27" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>177</v>
+      </c>
+      <c r="G27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>126</v>
       </c>
@@ -1397,8 +1585,14 @@
       <c r="E28" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>177</v>
+      </c>
+      <c r="G28" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>131</v>
       </c>
@@ -1414,8 +1608,14 @@
       <c r="E29" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>177</v>
+      </c>
+      <c r="G29" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>136</v>
       </c>
@@ -1431,8 +1631,14 @@
       <c r="E30" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>177</v>
+      </c>
+      <c r="G30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>141</v>
       </c>
@@ -1448,8 +1654,14 @@
       <c r="E31" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>177</v>
+      </c>
+      <c r="G31" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>146</v>
       </c>
@@ -1465,8 +1677,14 @@
       <c r="E32" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>177</v>
+      </c>
+      <c r="G32" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>151</v>
       </c>
@@ -1482,8 +1700,14 @@
       <c r="E33" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>177</v>
+      </c>
+      <c r="G33" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>156</v>
       </c>
@@ -1499,8 +1723,14 @@
       <c r="E34" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>177</v>
+      </c>
+      <c r="G34" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>160</v>
       </c>
@@ -1516,8 +1746,14 @@
       <c r="E35" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>177</v>
+      </c>
+      <c r="G35" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>165</v>
       </c>
@@ -1533,8 +1769,14 @@
       <c r="E36" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>177</v>
+      </c>
+      <c r="G36" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>169</v>
       </c>
@@ -1549,6 +1791,12 @@
       </c>
       <c r="E37" t="s">
         <v>173</v>
+      </c>
+      <c r="F37" t="s">
+        <v>177</v>
+      </c>
+      <c r="G37" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add engimon liar spawn
</commit_message>
<xml_diff>
--- a/data/Engimon.xlsx
+++ b/data/Engimon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STEI\Sem4\PBO\Nintendont-Game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C507E4B9-E491-4B59-9191-0D07DCCFB803}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE7BB7E-0FA2-42EA-A343-3EADE9E0003A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2220F236-1362-4FC8-8C2A-8F31A1E32F85}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="213">
   <si>
     <t>Name</t>
   </si>
@@ -580,6 +580,99 @@
   </si>
   <si>
     <t>Engimon/333.png</t>
+  </si>
+  <si>
+    <t>Engimon/077.png</t>
+  </si>
+  <si>
+    <t>Engimon/184.png</t>
+  </si>
+  <si>
+    <t>Engimon/148.png</t>
+  </si>
+  <si>
+    <t>Engimon/350.png</t>
+  </si>
+  <si>
+    <t>Engimon/446.png</t>
+  </si>
+  <si>
+    <t>Engimon/485.png</t>
+  </si>
+  <si>
+    <t>Engimon/479.png</t>
+  </si>
+  <si>
+    <t>Engimon/392s.png</t>
+  </si>
+  <si>
+    <t>Engimon/373.png</t>
+  </si>
+  <si>
+    <t>Engimon/378.png</t>
+  </si>
+  <si>
+    <t>Engimon/376.png</t>
+  </si>
+  <si>
+    <t>Engimon/381.png</t>
+  </si>
+  <si>
+    <t>Engimon/386.png</t>
+  </si>
+  <si>
+    <t>Engimon/310.png</t>
+  </si>
+  <si>
+    <t>Characters/boy_stand_south.png</t>
+  </si>
+  <si>
+    <t>Engimon/145.png</t>
+  </si>
+  <si>
+    <t>Engimon/160.png</t>
+  </si>
+  <si>
+    <t>Engimon/257.png</t>
+  </si>
+  <si>
+    <t>Engimon/275fs.png</t>
+  </si>
+  <si>
+    <t>Engimon/375.png</t>
+  </si>
+  <si>
+    <t>Engimon/377.png</t>
+  </si>
+  <si>
+    <t>Engimon/384.png</t>
+  </si>
+  <si>
+    <t>Engimon/488.png</t>
+  </si>
+  <si>
+    <t>Engimon/486.png</t>
+  </si>
+  <si>
+    <t>Engimon/623.png</t>
+  </si>
+  <si>
+    <t>Engimon/382.png</t>
+  </si>
+  <si>
+    <t>Engimon/643.png</t>
+  </si>
+  <si>
+    <t>Engimon/244.png</t>
+  </si>
+  <si>
+    <t>Engimon/445.png</t>
+  </si>
+  <si>
+    <t>Engimon/448s.png</t>
+  </si>
+  <si>
+    <t>Engimon/065fs.png</t>
   </si>
 </sst>
 </file>
@@ -933,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAA2AB0-BD4B-4942-9DAC-0BAE7234D902}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +1084,7 @@
         <v>176</v>
       </c>
       <c r="G2" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1014,7 +1107,7 @@
         <v>181</v>
       </c>
       <c r="G3" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1037,7 +1130,7 @@
         <v>179</v>
       </c>
       <c r="G4" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1060,7 +1153,7 @@
         <v>180</v>
       </c>
       <c r="G5" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1083,7 +1176,7 @@
         <v>178</v>
       </c>
       <c r="G6" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1103,10 +1196,10 @@
         <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="G7" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1126,10 +1219,10 @@
         <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="G8" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1149,10 +1242,10 @@
         <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="G9" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1172,10 +1265,10 @@
         <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="G10" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1195,10 +1288,10 @@
         <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="G11" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1218,10 +1311,10 @@
         <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="G12" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1241,10 +1334,10 @@
         <v>58</v>
       </c>
       <c r="F13" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="G13" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1264,10 +1357,10 @@
         <v>63</v>
       </c>
       <c r="F14" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="G14" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1287,10 +1380,10 @@
         <v>68</v>
       </c>
       <c r="F15" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="G15" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1310,10 +1403,10 @@
         <v>73</v>
       </c>
       <c r="F16" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="G16" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1333,10 +1426,10 @@
         <v>78</v>
       </c>
       <c r="F17" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="G17" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1356,10 +1449,10 @@
         <v>82</v>
       </c>
       <c r="F18" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="G18" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1379,10 +1472,10 @@
         <v>87</v>
       </c>
       <c r="F19" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="G19" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1402,10 +1495,10 @@
         <v>92</v>
       </c>
       <c r="F20" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="G20" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1425,10 +1518,10 @@
         <v>97</v>
       </c>
       <c r="F21" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="G21" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1448,10 +1541,10 @@
         <v>101</v>
       </c>
       <c r="F22" t="s">
-        <v>177</v>
+        <v>198</v>
       </c>
       <c r="G22" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1471,10 +1564,10 @@
         <v>105</v>
       </c>
       <c r="F23" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="G23" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1494,10 +1587,10 @@
         <v>110</v>
       </c>
       <c r="F24" t="s">
-        <v>177</v>
+        <v>200</v>
       </c>
       <c r="G24" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1517,10 +1610,10 @@
         <v>115</v>
       </c>
       <c r="F25" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="G25" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1540,10 +1633,10 @@
         <v>120</v>
       </c>
       <c r="F26" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="G26" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1563,10 +1656,10 @@
         <v>125</v>
       </c>
       <c r="F27" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
       <c r="G27" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1586,10 +1679,10 @@
         <v>130</v>
       </c>
       <c r="F28" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="G28" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1609,10 +1702,10 @@
         <v>135</v>
       </c>
       <c r="F29" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="G29" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1632,10 +1725,10 @@
         <v>140</v>
       </c>
       <c r="F30" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="G30" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1655,10 +1748,10 @@
         <v>145</v>
       </c>
       <c r="F31" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="G31" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1678,10 +1771,10 @@
         <v>150</v>
       </c>
       <c r="F32" t="s">
-        <v>177</v>
+        <v>208</v>
       </c>
       <c r="G32" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1701,10 +1794,10 @@
         <v>155</v>
       </c>
       <c r="F33" t="s">
-        <v>177</v>
+        <v>211</v>
       </c>
       <c r="G33" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1724,10 +1817,10 @@
         <v>159</v>
       </c>
       <c r="F34" t="s">
-        <v>177</v>
+        <v>210</v>
       </c>
       <c r="G34" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1750,7 +1843,7 @@
         <v>177</v>
       </c>
       <c r="G35" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1770,10 +1863,10 @@
         <v>168</v>
       </c>
       <c r="F36" t="s">
-        <v>177</v>
+        <v>209</v>
       </c>
       <c r="G36" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1793,10 +1886,10 @@
         <v>173</v>
       </c>
       <c r="F37" t="s">
-        <v>177</v>
+        <v>212</v>
       </c>
       <c r="G37" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spawn engimon liar, restyle starting menu, active engimon
</commit_message>
<xml_diff>
--- a/data/Engimon.xlsx
+++ b/data/Engimon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STEI\Sem4\PBO\Nintendont-Game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE7BB7E-0FA2-42EA-A343-3EADE9E0003A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820F1143-1470-4197-9379-05296BB7C10F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2220F236-1362-4FC8-8C2A-8F31A1E32F85}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="215">
   <si>
     <t>Name</t>
   </si>
@@ -624,9 +624,6 @@
     <t>Engimon/310.png</t>
   </si>
   <si>
-    <t>Characters/boy_stand_south.png</t>
-  </si>
-  <si>
     <t>Engimon/145.png</t>
   </si>
   <si>
@@ -673,6 +670,15 @@
   </si>
   <si>
     <t>Engimon/065fs.png</t>
+  </si>
+  <si>
+    <t>Icons/icon004.png</t>
+  </si>
+  <si>
+    <t>Icons/icon333.png</t>
+  </si>
+  <si>
+    <t>Icons/icon011.png</t>
   </si>
 </sst>
 </file>
@@ -1026,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAA2AB0-BD4B-4942-9DAC-0BAE7234D902}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,7 +1090,7 @@
         <v>176</v>
       </c>
       <c r="G2" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1107,7 +1113,7 @@
         <v>181</v>
       </c>
       <c r="G3" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1130,7 +1136,7 @@
         <v>179</v>
       </c>
       <c r="G4" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1153,7 +1159,7 @@
         <v>180</v>
       </c>
       <c r="G5" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1176,7 +1182,7 @@
         <v>178</v>
       </c>
       <c r="G6" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1199,7 +1205,7 @@
         <v>182</v>
       </c>
       <c r="G7" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1222,7 +1228,7 @@
         <v>184</v>
       </c>
       <c r="G8" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1245,7 +1251,7 @@
         <v>185</v>
       </c>
       <c r="G9" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1268,7 +1274,7 @@
         <v>186</v>
       </c>
       <c r="G10" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1291,7 +1297,7 @@
         <v>183</v>
       </c>
       <c r="G11" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1314,7 +1320,7 @@
         <v>189</v>
       </c>
       <c r="G12" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1337,7 +1343,7 @@
         <v>187</v>
       </c>
       <c r="G13" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1360,7 +1366,7 @@
         <v>188</v>
       </c>
       <c r="G14" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1383,7 +1389,7 @@
         <v>190</v>
       </c>
       <c r="G15" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1406,7 +1412,7 @@
         <v>192</v>
       </c>
       <c r="G16" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1429,7 +1435,7 @@
         <v>191</v>
       </c>
       <c r="G17" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1452,7 +1458,7 @@
         <v>193</v>
       </c>
       <c r="G18" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1475,7 +1481,7 @@
         <v>194</v>
       </c>
       <c r="G19" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1498,7 +1504,7 @@
         <v>195</v>
       </c>
       <c r="G20" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1518,10 +1524,10 @@
         <v>97</v>
       </c>
       <c r="F21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G21" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1541,10 +1547,10 @@
         <v>101</v>
       </c>
       <c r="F22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G22" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1564,10 +1570,10 @@
         <v>105</v>
       </c>
       <c r="F23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G23" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1587,10 +1593,10 @@
         <v>110</v>
       </c>
       <c r="F24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G24" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1610,10 +1616,10 @@
         <v>115</v>
       </c>
       <c r="F25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G25" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1633,10 +1639,10 @@
         <v>120</v>
       </c>
       <c r="F26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G26" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1656,10 +1662,10 @@
         <v>125</v>
       </c>
       <c r="F27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G27" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1679,10 +1685,10 @@
         <v>130</v>
       </c>
       <c r="F28" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G28" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1702,10 +1708,10 @@
         <v>135</v>
       </c>
       <c r="F29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G29" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1725,10 +1731,10 @@
         <v>140</v>
       </c>
       <c r="F30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G30" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1748,10 +1754,10 @@
         <v>145</v>
       </c>
       <c r="F31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G31" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1771,10 +1777,10 @@
         <v>150</v>
       </c>
       <c r="F32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G32" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1794,10 +1800,10 @@
         <v>155</v>
       </c>
       <c r="F33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G33" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1817,10 +1823,10 @@
         <v>159</v>
       </c>
       <c r="F34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G34" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1843,7 +1849,7 @@
         <v>177</v>
       </c>
       <c r="G35" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1863,10 +1869,10 @@
         <v>168</v>
       </c>
       <c r="F36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G36" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1886,10 +1892,10 @@
         <v>173</v>
       </c>
       <c r="F37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G37" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix active engimon position
</commit_message>
<xml_diff>
--- a/data/Engimon.xlsx
+++ b/data/Engimon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STEI\Sem4\PBO\Nintendont-Game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820F1143-1470-4197-9379-05296BB7C10F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531A3BC6-7318-4945-A1E8-EE21CFA6692B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2220F236-1362-4FC8-8C2A-8F31A1E32F85}"/>
+    <workbookView xWindow="-29530" yWindow="-2740" windowWidth="30630" windowHeight="16640" xr2:uid="{2220F236-1362-4FC8-8C2A-8F31A1E32F85}"/>
   </bookViews>
   <sheets>
     <sheet name="EngimonList" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="248">
   <si>
     <t>Name</t>
   </si>
@@ -679,6 +679,105 @@
   </si>
   <si>
     <t>Icons/icon011.png</t>
+  </si>
+  <si>
+    <t>Icons/icon053.png</t>
+  </si>
+  <si>
+    <t>Icons/icon007.png</t>
+  </si>
+  <si>
+    <t>Icons/icon077.png</t>
+  </si>
+  <si>
+    <t>Icons/icon148.png</t>
+  </si>
+  <si>
+    <t>Icons/icon350.png</t>
+  </si>
+  <si>
+    <t>Icons/icon446.png</t>
+  </si>
+  <si>
+    <t>Icons/icon184.png</t>
+  </si>
+  <si>
+    <t>Icons/icon392.png</t>
+  </si>
+  <si>
+    <t>Icons/icon485.png</t>
+  </si>
+  <si>
+    <t>Icons/icon479.png</t>
+  </si>
+  <si>
+    <t>Icons/icon373.png</t>
+  </si>
+  <si>
+    <t>Icons/icon376.png</t>
+  </si>
+  <si>
+    <t>Icons/icon378.png</t>
+  </si>
+  <si>
+    <t>Icons/icon381.png</t>
+  </si>
+  <si>
+    <t>Icons/icon386.png</t>
+  </si>
+  <si>
+    <t>Icons/icon310.png</t>
+  </si>
+  <si>
+    <t>Icons/icon145.png</t>
+  </si>
+  <si>
+    <t>Icons/icon160.png</t>
+  </si>
+  <si>
+    <t>Icons/icon257.png</t>
+  </si>
+  <si>
+    <t>Icons/icon275.png</t>
+  </si>
+  <si>
+    <t>Icons/icon375.png</t>
+  </si>
+  <si>
+    <t>Icons/icon377.png</t>
+  </si>
+  <si>
+    <t>Icons/icon384.png</t>
+  </si>
+  <si>
+    <t>Icons/icon488.png</t>
+  </si>
+  <si>
+    <t>Icons/icon486.png</t>
+  </si>
+  <si>
+    <t>Icons/icon623.png</t>
+  </si>
+  <si>
+    <t>Icons/icon382.png</t>
+  </si>
+  <si>
+    <t>Icons/icon643.png</t>
+  </si>
+  <si>
+    <t>Icons/icon448.png</t>
+  </si>
+  <si>
+    <t>Icons/icon445.png</t>
+  </si>
+  <si>
+    <t>Icons/icon000.png</t>
+  </si>
+  <si>
+    <t>Icons/icon244.png</t>
+  </si>
+  <si>
+    <t>Icons/icon065.png</t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1132,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,7 +1258,7 @@
         <v>180</v>
       </c>
       <c r="G5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1182,7 +1281,7 @@
         <v>178</v>
       </c>
       <c r="G6" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1205,7 +1304,7 @@
         <v>182</v>
       </c>
       <c r="G7" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1228,7 +1327,7 @@
         <v>184</v>
       </c>
       <c r="G8" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1251,7 +1350,7 @@
         <v>185</v>
       </c>
       <c r="G9" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1274,7 +1373,7 @@
         <v>186</v>
       </c>
       <c r="G10" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1297,7 +1396,7 @@
         <v>183</v>
       </c>
       <c r="G11" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1320,7 +1419,7 @@
         <v>189</v>
       </c>
       <c r="G12" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1343,7 +1442,7 @@
         <v>187</v>
       </c>
       <c r="G13" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1366,7 +1465,7 @@
         <v>188</v>
       </c>
       <c r="G14" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1389,7 +1488,7 @@
         <v>190</v>
       </c>
       <c r="G15" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1412,7 +1511,7 @@
         <v>192</v>
       </c>
       <c r="G16" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1435,7 +1534,7 @@
         <v>191</v>
       </c>
       <c r="G17" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1458,7 +1557,7 @@
         <v>193</v>
       </c>
       <c r="G18" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1481,7 +1580,7 @@
         <v>194</v>
       </c>
       <c r="G19" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1504,7 +1603,7 @@
         <v>195</v>
       </c>
       <c r="G20" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1527,7 +1626,7 @@
         <v>196</v>
       </c>
       <c r="G21" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1550,7 +1649,7 @@
         <v>197</v>
       </c>
       <c r="G22" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1573,7 +1672,7 @@
         <v>198</v>
       </c>
       <c r="G23" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1596,7 +1695,7 @@
         <v>199</v>
       </c>
       <c r="G24" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1619,7 +1718,7 @@
         <v>200</v>
       </c>
       <c r="G25" t="s">
-        <v>214</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1642,7 +1741,7 @@
         <v>201</v>
       </c>
       <c r="G26" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1665,7 +1764,7 @@
         <v>202</v>
       </c>
       <c r="G27" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1688,7 +1787,7 @@
         <v>203</v>
       </c>
       <c r="G28" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1711,7 +1810,7 @@
         <v>204</v>
       </c>
       <c r="G29" t="s">
-        <v>214</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1734,7 +1833,7 @@
         <v>205</v>
       </c>
       <c r="G30" t="s">
-        <v>214</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1757,7 +1856,7 @@
         <v>206</v>
       </c>
       <c r="G31" t="s">
-        <v>214</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1780,7 +1879,7 @@
         <v>207</v>
       </c>
       <c r="G32" t="s">
-        <v>214</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1803,7 +1902,7 @@
         <v>210</v>
       </c>
       <c r="G33" t="s">
-        <v>214</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1826,7 +1925,7 @@
         <v>209</v>
       </c>
       <c r="G34" t="s">
-        <v>214</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1849,7 +1948,7 @@
         <v>177</v>
       </c>
       <c r="G35" t="s">
-        <v>214</v>
+        <v>245</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1872,7 +1971,7 @@
         <v>208</v>
       </c>
       <c r="G36" t="s">
-        <v>214</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1895,7 +1994,7 @@
         <v>211</v>
       </c>
       <c r="G37" t="s">
-        <v>214</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>